<commit_message>
Fixed legend not visible
</commit_message>
<xml_diff>
--- a/filer/diagram-mall.xlsx
+++ b/filer/diagram-mall.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{542918ED-1675-40FC-A09D-BBBEB89B95D6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9AE012F-DB88-43D0-A483-626F0675B177}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10440" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11400" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Paj" sheetId="5" r:id="rId1"/>
@@ -344,19 +344,22 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -369,9 +372,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -436,7 +436,17 @@
           </a:p>
           <a:p>
             <a:pPr algn="l">
-              <a:defRPr/>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
             </a:pPr>
             <a:r>
               <a:rPr lang="sv-SE" sz="1000" b="0" baseline="0"/>
@@ -462,26 +472,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l">
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="sv-SE"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -555,13 +545,18 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-81A5-460F-B459-7459F3004CD9}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.15227469129032972"/>
+                  <c:x val="-0.12627654830054327"/>
                   <c:y val="6.2424478309032666E-2"/>
                 </c:manualLayout>
               </c:layout>
@@ -605,14 +600,10 @@
                     <a:prstGeom prst="rect">
                       <a:avLst/>
                     </a:prstGeom>
-                    <a:noFill/>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
                   </c15:spPr>
                   <c15:layout>
                     <c:manualLayout>
-                      <c:w val="0.30640668523676878"/>
+                      <c:w val="0.35840297121634168"/>
                       <c:h val="0.23288973384030418"/>
                     </c:manualLayout>
                   </c15:layout>
@@ -664,20 +655,77 @@
                     <a:prstGeom prst="rect">
                       <a:avLst/>
                     </a:prstGeom>
-                    <a:noFill/>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
                   </c15:spPr>
                   <c15:layout>
                     <c:manualLayout>
-                      <c:w val="0.35468895078922935"/>
-                      <c:h val="0.19866920152091255"/>
+                      <c:w val="0.30588672237697312"/>
+                      <c:h val="0.16887847669231459"/>
                     </c:manualLayout>
                   </c15:layout>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-C1E7-4AD8-9151-8FA20A02DF58}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.10770659238625808"/>
+                  <c:y val="0.15304182509505704"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:noAutofit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:sysClr val="windowText" lastClr="000000"/>
+                      </a:solidFill>
+                      <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="sv-SE"/>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:separator>
+</c:separator>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <a:prstGeom prst="rect">
+                      <a:avLst/>
+                    </a:prstGeom>
+                  </c15:spPr>
+                  <c15:layout>
+                    <c:manualLayout>
+                      <c:w val="0.22376973073351902"/>
+                      <c:h val="0.20532319391634982"/>
+                    </c:manualLayout>
+                  </c15:layout>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-81A5-460F-B459-7459F3004CD9}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -722,10 +770,6 @@
                   <a:prstGeom prst="rect">
                     <a:avLst/>
                   </a:prstGeom>
-                  <a:noFill/>
-                  <a:ln>
-                    <a:noFill/>
-                  </a:ln>
                 </c15:spPr>
               </c:ext>
             </c:extLst>
@@ -1367,7 +1411,7 @@
             </a:br>
             <a:r>
               <a:rPr lang="sv-SE" sz="1000" b="0"/>
-              <a:t>Procent</a:t>
+              <a:t>Procent (n = 1 516)</a:t>
             </a:r>
             <a:endParaRPr lang="sv-SE" b="0"/>
           </a:p>
@@ -1920,7 +1964,7 @@
             </a:br>
             <a:r>
               <a:rPr lang="sv-SE" sz="1000" b="0"/>
-              <a:t>Procent</a:t>
+              <a:t>Procent (n = 1 516)</a:t>
             </a:r>
             <a:endParaRPr lang="sv-SE" b="0"/>
           </a:p>
@@ -2460,9 +2504,9 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.33055752405949257"/>
+          <c:x val="0.23889085739282589"/>
           <c:y val="0.93661390933516253"/>
-          <c:w val="0.33888495188101486"/>
+          <c:w val="0.58610717410323709"/>
           <c:h val="6.3386090664837511E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -2579,7 +2623,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="sv-SE" sz="1000"/>
-              <a:t>Procent</a:t>
+              <a:t>Procent (n = 1 516)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -6756,48 +6800,8 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -6854,7 +6858,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -6905,13 +6909,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050">
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -6922,19 +6919,12 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="25400">
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
+    <cs:fillRef idx="1"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
@@ -6972,7 +6962,7 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
+    <cs:fillRef idx="1"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
@@ -7015,23 +7005,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -7136,8 +7125,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -7269,20 +7258,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -8825,7 +8813,7 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -9029,22 +9017,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -9149,8 +9138,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -9282,19 +9271,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -9833,7 +9823,7 @@
 </file>
 
 <file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -10338,511 +10328,6 @@
 </file>
 
 <file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -12047,46 +11532,46 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -12207,18 +11692,18 @@
       </c>
     </row>
     <row r="28" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29" s="7"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
+      <c r="A29" s="8"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
     </row>
     <row r="44" spans="1:3" ht="25" x14ac:dyDescent="0.5">
       <c r="A44" s="5" t="s">
@@ -12278,36 +11763,36 @@
       <c r="C51" s="4"/>
     </row>
     <row r="52" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="8" t="s">
+      <c r="A52" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B52" s="8"/>
-      <c r="C52" s="8"/>
-      <c r="D52" s="8"/>
+      <c r="B52" s="7"/>
+      <c r="C52" s="7"/>
+      <c r="D52" s="7"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A53" s="8"/>
-      <c r="B53" s="8"/>
-      <c r="C53" s="8"/>
-      <c r="D53" s="8"/>
+      <c r="A53" s="7"/>
+      <c r="B53" s="7"/>
+      <c r="C53" s="7"/>
+      <c r="D53" s="7"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A54" s="8"/>
-      <c r="B54" s="8"/>
-      <c r="C54" s="8"/>
-      <c r="D54" s="8"/>
+      <c r="A54" s="7"/>
+      <c r="B54" s="7"/>
+      <c r="C54" s="7"/>
+      <c r="D54" s="7"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A55" s="8"/>
-      <c r="B55" s="8"/>
-      <c r="C55" s="8"/>
-      <c r="D55" s="8"/>
+      <c r="A55" s="7"/>
+      <c r="B55" s="7"/>
+      <c r="C55" s="7"/>
+      <c r="D55" s="7"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A56" s="8"/>
-      <c r="B56" s="8"/>
-      <c r="C56" s="8"/>
-      <c r="D56" s="8"/>
+      <c r="A56" s="7"/>
+      <c r="B56" s="7"/>
+      <c r="C56" s="7"/>
+      <c r="D56" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -12324,7 +11809,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F64"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AA51" sqref="AA51"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -12464,26 +11951,26 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
     </row>
     <row r="24" spans="1:5" ht="25" x14ac:dyDescent="0.5">
       <c r="A24" s="5" t="s">
@@ -12579,21 +12066,21 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A35" s="6" t="s">
+      <c r="A35" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B35" s="15"/>
-      <c r="C35" s="15"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A36" s="15"/>
-      <c r="B36" s="15"/>
-      <c r="C36" s="15"/>
+      <c r="A36" s="10"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A37" s="15"/>
-      <c r="B37" s="15"/>
-      <c r="C37" s="15"/>
+      <c r="A37" s="10"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
     </row>
     <row r="46" spans="1:3" ht="25" x14ac:dyDescent="0.5">
       <c r="A46" s="5" t="s">
@@ -12662,30 +12149,30 @@
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A59" s="9" t="s">
+      <c r="A59" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="B59" s="11"/>
+      <c r="B59" s="12"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A60" s="7"/>
-      <c r="B60" s="12"/>
+      <c r="A60" s="8"/>
+      <c r="B60" s="13"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A61" s="7"/>
-      <c r="B61" s="12"/>
+      <c r="A61" s="8"/>
+      <c r="B61" s="13"/>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A62" s="7"/>
-      <c r="B62" s="12"/>
+      <c r="A62" s="8"/>
+      <c r="B62" s="13"/>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A63" s="7"/>
-      <c r="B63" s="12"/>
+      <c r="A63" s="8"/>
+      <c r="B63" s="13"/>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A64" s="13"/>
-      <c r="B64" s="14"/>
+      <c r="A64" s="14"/>
+      <c r="B64" s="15"/>
     </row>
   </sheetData>
   <sortState ref="B28:D32">
@@ -12991,21 +12478,21 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A42" s="6" t="s">
+      <c r="A42" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B42" s="6"/>
-      <c r="C42" s="6"/>
+      <c r="B42" s="9"/>
+      <c r="C42" s="9"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A43" s="6"/>
-      <c r="B43" s="6"/>
-      <c r="C43" s="6"/>
+      <c r="A43" s="9"/>
+      <c r="B43" s="9"/>
+      <c r="C43" s="9"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A44" s="6"/>
-      <c r="B44" s="6"/>
-      <c r="C44" s="6"/>
+      <c r="A44" s="9"/>
+      <c r="B44" s="9"/>
+      <c r="C44" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>